<commit_message>
Refactor: Cleaning the code
</commit_message>
<xml_diff>
--- a/BTC raport - 27.04.2023.xlsx
+++ b/BTC raport - 27.04.2023.xlsx
@@ -448,7 +448,7 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Raport BTC - 27.04.2023 00:46:52</t>
+          <t>Raport BTC - 27.04.2023 01:54:23</t>
         </is>
       </c>
     </row>
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28341.2</v>
+        <v>28367.3</v>
       </c>
       <c r="D35" t="n">
         <v>28298.8</v>

</xml_diff>